<commit_message>
🔄 Actualización automática del mapa (mapa_interactivo.html)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P413"/>
+  <dimension ref="A1:P412"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29041,7 +29041,7 @@
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>-500</t>
+          <t>6330</t>
         </is>
       </c>
       <c r="B384" t="inlineStr">
@@ -29051,22 +29051,22 @@
       </c>
       <c r="C384" t="inlineStr">
         <is>
-          <t>Castañares 5656</t>
+          <t>REPUBLICA DE LA INDIA 3106</t>
         </is>
       </c>
       <c r="D384" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E384" t="inlineStr">
         <is>
-          <t>807965768</t>
+          <t>807965776</t>
         </is>
       </c>
       <c r="F384" t="inlineStr">
         <is>
-          <t>AYKO</t>
+          <t>Optical Power</t>
         </is>
       </c>
       <c r="G384" t="inlineStr">
@@ -29076,7 +29076,7 @@
       </c>
       <c r="H384" t="inlineStr">
         <is>
-          <t>Columna chocada con rienda a pique</t>
+          <t>Picada e inclinada</t>
         </is>
       </c>
       <c r="I384" t="n">
@@ -29094,18 +29094,18 @@
       </c>
       <c r="L384" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M384" t="n">
-        <v>-58.479921</v>
+        <v>-58.413941</v>
       </c>
       <c r="N384" t="n">
-        <v>-34.673021</v>
+        <v>-34.57698</v>
       </c>
       <c r="O384" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P384" t="inlineStr">
@@ -29117,7 +29117,7 @@
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>6330</t>
+          <t>6331</t>
         </is>
       </c>
       <c r="B385" t="inlineStr">
@@ -29127,7 +29127,7 @@
       </c>
       <c r="C385" t="inlineStr">
         <is>
-          <t>REPUBLICA DE LA INDIA 3106</t>
+          <t>PARAGUAY 4259</t>
         </is>
       </c>
       <c r="D385" t="inlineStr">
@@ -29137,12 +29137,12 @@
       </c>
       <c r="E385" t="inlineStr">
         <is>
-          <t>807965776</t>
+          <t>807965788</t>
         </is>
       </c>
       <c r="F385" t="inlineStr">
         <is>
-          <t>Optical Power</t>
+          <t>NEW</t>
         </is>
       </c>
       <c r="G385" t="inlineStr">
@@ -29152,7 +29152,7 @@
       </c>
       <c r="H385" t="inlineStr">
         <is>
-          <t>Picada e inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I385" t="n">
@@ -29174,10 +29174,10 @@
         </is>
       </c>
       <c r="M385" t="n">
-        <v>-58.413941</v>
+        <v>-58.421822</v>
       </c>
       <c r="N385" t="n">
-        <v>-34.57698</v>
+        <v>-34.58645</v>
       </c>
       <c r="O385" t="inlineStr">
         <is>
@@ -29193,7 +29193,7 @@
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>6331</t>
+          <t>6332</t>
         </is>
       </c>
       <c r="B386" t="inlineStr">
@@ -29203,7 +29203,7 @@
       </c>
       <c r="C386" t="inlineStr">
         <is>
-          <t>PARAGUAY 4259</t>
+          <t>ARAOZ 2560</t>
         </is>
       </c>
       <c r="D386" t="inlineStr">
@@ -29213,7 +29213,7 @@
       </c>
       <c r="E386" t="inlineStr">
         <is>
-          <t>807965788</t>
+          <t>807965818</t>
         </is>
       </c>
       <c r="F386" t="inlineStr">
@@ -29250,10 +29250,10 @@
         </is>
       </c>
       <c r="M386" t="n">
-        <v>-58.421822</v>
+        <v>-58.414507</v>
       </c>
       <c r="N386" t="n">
-        <v>-34.58645</v>
+        <v>-34.585377</v>
       </c>
       <c r="O386" t="inlineStr">
         <is>
@@ -29269,7 +29269,7 @@
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>6332</t>
+          <t>6336</t>
         </is>
       </c>
       <c r="B387" t="inlineStr">
@@ -29279,7 +29279,7 @@
       </c>
       <c r="C387" t="inlineStr">
         <is>
-          <t>ARAOZ 2560</t>
+          <t>PARAGUAY 4291</t>
         </is>
       </c>
       <c r="D387" t="inlineStr">
@@ -29289,7 +29289,7 @@
       </c>
       <c r="E387" t="inlineStr">
         <is>
-          <t>807965818</t>
+          <t>807965819</t>
         </is>
       </c>
       <c r="F387" t="inlineStr">
@@ -29326,10 +29326,10 @@
         </is>
       </c>
       <c r="M387" t="n">
-        <v>-58.414507</v>
+        <v>-58.422084</v>
       </c>
       <c r="N387" t="n">
-        <v>-34.585377</v>
+        <v>-34.58625</v>
       </c>
       <c r="O387" t="inlineStr">
         <is>
@@ -29345,7 +29345,7 @@
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
-          <t>6336</t>
+          <t>6337</t>
         </is>
       </c>
       <c r="B388" t="inlineStr">
@@ -29355,7 +29355,7 @@
       </c>
       <c r="C388" t="inlineStr">
         <is>
-          <t>PARAGUAY 4291</t>
+          <t>PARAGUAY 4383</t>
         </is>
       </c>
       <c r="D388" t="inlineStr">
@@ -29365,7 +29365,7 @@
       </c>
       <c r="E388" t="inlineStr">
         <is>
-          <t>807965819</t>
+          <t>807965926</t>
         </is>
       </c>
       <c r="F388" t="inlineStr">
@@ -29402,10 +29402,10 @@
         </is>
       </c>
       <c r="M388" t="n">
-        <v>-58.422084</v>
+        <v>-58.422931</v>
       </c>
       <c r="N388" t="n">
-        <v>-34.58625</v>
+        <v>-34.585597</v>
       </c>
       <c r="O388" t="inlineStr">
         <is>
@@ -29421,7 +29421,7 @@
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>6337</t>
+          <t>-501</t>
         </is>
       </c>
       <c r="B389" t="inlineStr">
@@ -29431,7 +29431,7 @@
       </c>
       <c r="C389" t="inlineStr">
         <is>
-          <t>PARAGUAY 4383</t>
+          <t>Cabello 3107</t>
         </is>
       </c>
       <c r="D389" t="inlineStr">
@@ -29441,12 +29441,12 @@
       </c>
       <c r="E389" t="inlineStr">
         <is>
-          <t>807965926</t>
+          <t>807971967</t>
         </is>
       </c>
       <c r="F389" t="inlineStr">
         <is>
-          <t>NEW</t>
+          <t>Optical Power</t>
         </is>
       </c>
       <c r="G389" t="inlineStr">
@@ -29456,15 +29456,15 @@
       </c>
       <c r="H389" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I389" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J389" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K389" t="inlineStr">
@@ -29474,18 +29474,18 @@
       </c>
       <c r="L389" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M389" t="n">
-        <v>-58.422931</v>
+        <v>-58.405749</v>
       </c>
       <c r="N389" t="n">
-        <v>-34.585597</v>
+        <v>-34.58224</v>
       </c>
       <c r="O389" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P389" t="inlineStr">
@@ -29497,27 +29497,27 @@
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t>-501</t>
+          <t>6357</t>
         </is>
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/7/2025</t>
         </is>
       </c>
       <c r="C390" t="inlineStr">
         <is>
-          <t>Cabello 3107</t>
+          <t>BACACAY 3088</t>
         </is>
       </c>
       <c r="D390" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E390" t="inlineStr">
         <is>
-          <t>807971967</t>
+          <t>808036196</t>
         </is>
       </c>
       <c r="F390" t="inlineStr">
@@ -29532,15 +29532,15 @@
       </c>
       <c r="H390" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I390" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J390" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K390" t="inlineStr">
@@ -29554,26 +29554,26 @@
         </is>
       </c>
       <c r="M390" t="n">
-        <v>-58.405749</v>
+        <v>-58.473179</v>
       </c>
       <c r="N390" t="n">
-        <v>-34.58224</v>
+        <v>-34.629138</v>
       </c>
       <c r="O390" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P390" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="inlineStr">
         <is>
-          <t>6357</t>
+          <t>-502</t>
         </is>
       </c>
       <c r="B391" t="inlineStr">
@@ -29583,17 +29583,17 @@
       </c>
       <c r="C391" t="inlineStr">
         <is>
-          <t>BACACAY 3088</t>
+          <t>Tagle 2562</t>
         </is>
       </c>
       <c r="D391" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E391" t="inlineStr">
         <is>
-          <t>808036196</t>
+          <t>808036198</t>
         </is>
       </c>
       <c r="F391" t="inlineStr">
@@ -29608,7 +29608,7 @@
       </c>
       <c r="H391" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Colocar columna para pedir traspaso nodo teco</t>
         </is>
       </c>
       <c r="I391" t="n">
@@ -29616,65 +29616,65 @@
       </c>
       <c r="J391" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K391" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L391" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M391" t="n">
-        <v>-58.473179</v>
+        <v>-58.400188</v>
       </c>
       <c r="N391" t="n">
-        <v>-34.629138</v>
+        <v>-34.583882</v>
       </c>
       <c r="O391" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P391" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="inlineStr">
         <is>
-          <t>-502</t>
+          <t>6363</t>
         </is>
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>7/7/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C392" t="inlineStr">
         <is>
-          <t>Tagle 2562</t>
+          <t>MOLDES 3730</t>
         </is>
       </c>
       <c r="D392" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E392" t="inlineStr">
         <is>
-          <t>808036198</t>
+          <t>808099415</t>
         </is>
       </c>
       <c r="F392" t="inlineStr">
         <is>
-          <t>Optical Power</t>
+          <t>NEW</t>
         </is>
       </c>
       <c r="G392" t="inlineStr">
@@ -29684,7 +29684,7 @@
       </c>
       <c r="H392" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso nodo teco</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I392" t="n">
@@ -29692,40 +29692,40 @@
       </c>
       <c r="J392" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K392" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L392" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M392" t="n">
-        <v>-58.400188</v>
+        <v>-58.47192</v>
       </c>
       <c r="N392" t="n">
-        <v>-34.583882</v>
+        <v>-34.549398</v>
       </c>
       <c r="O392" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P392" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t>6363</t>
+          <t>6376</t>
         </is>
       </c>
       <c r="B393" t="inlineStr">
@@ -29735,22 +29735,22 @@
       </c>
       <c r="C393" t="inlineStr">
         <is>
-          <t>MOLDES 3730</t>
+          <t>BOYACA 712</t>
         </is>
       </c>
       <c r="D393" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E393" t="inlineStr">
         <is>
-          <t>808099415</t>
+          <t>808099366</t>
         </is>
       </c>
       <c r="F393" t="inlineStr">
         <is>
-          <t>NEW</t>
+          <t>PEBCOM</t>
         </is>
       </c>
       <c r="G393" t="inlineStr">
@@ -29760,7 +29760,7 @@
       </c>
       <c r="H393" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I393" t="n">
@@ -29768,7 +29768,7 @@
       </c>
       <c r="J393" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K393" t="inlineStr">
@@ -29778,30 +29778,30 @@
       </c>
       <c r="L393" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M393" t="n">
-        <v>-58.47192</v>
+        <v>-58.461858</v>
       </c>
       <c r="N393" t="n">
-        <v>-34.549398</v>
+        <v>-34.619348</v>
       </c>
       <c r="O393" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P393" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>6376</t>
+          <t>6377</t>
         </is>
       </c>
       <c r="B394" t="inlineStr">
@@ -29811,22 +29811,22 @@
       </c>
       <c r="C394" t="inlineStr">
         <is>
-          <t>BOYACA 712</t>
+          <t>GUARDIA VIEJA 4377</t>
         </is>
       </c>
       <c r="D394" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E394" t="inlineStr">
         <is>
-          <t>808099366</t>
+          <t>808099347</t>
         </is>
       </c>
       <c r="F394" t="inlineStr">
         <is>
-          <t>PEBCOM</t>
+          <t>Optical Power</t>
         </is>
       </c>
       <c r="G394" t="inlineStr">
@@ -29858,14 +29858,14 @@
         </is>
       </c>
       <c r="M394" t="n">
-        <v>-58.461858</v>
+        <v>-58.426322</v>
       </c>
       <c r="N394" t="n">
-        <v>-34.619348</v>
+        <v>-34.600097</v>
       </c>
       <c r="O394" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P394" t="inlineStr">
@@ -29877,7 +29877,7 @@
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t>6377</t>
+          <t>6383</t>
         </is>
       </c>
       <c r="B395" t="inlineStr">
@@ -29887,17 +29887,17 @@
       </c>
       <c r="C395" t="inlineStr">
         <is>
-          <t>GUARDIA VIEJA 4377</t>
+          <t>FALCON, RAMON L.,CNEL. 1411</t>
         </is>
       </c>
       <c r="D395" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E395" t="inlineStr">
         <is>
-          <t>808099347</t>
+          <t>808099320</t>
         </is>
       </c>
       <c r="F395" t="inlineStr">
@@ -29934,14 +29934,14 @@
         </is>
       </c>
       <c r="M395" t="n">
-        <v>-58.426322</v>
+        <v>-58.448523</v>
       </c>
       <c r="N395" t="n">
-        <v>-34.600097</v>
+        <v>-34.62452</v>
       </c>
       <c r="O395" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P395" t="inlineStr">
@@ -29953,32 +29953,32 @@
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>6383</t>
+          <t>-503</t>
         </is>
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C396" t="inlineStr">
         <is>
-          <t>FALCON, RAMON L.,CNEL. 1411</t>
+          <t>Salguero 842</t>
         </is>
       </c>
       <c r="D396" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E396" t="inlineStr">
         <is>
-          <t>808099320</t>
+          <t>808148673</t>
         </is>
       </c>
       <c r="F396" t="inlineStr">
         <is>
-          <t>Optical Power</t>
+          <t>NEW</t>
         </is>
       </c>
       <c r="G396" t="inlineStr">
@@ -29988,7 +29988,7 @@
       </c>
       <c r="H396" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna picada en la base</t>
         </is>
       </c>
       <c r="I396" t="n">
@@ -30010,14 +30010,14 @@
         </is>
       </c>
       <c r="M396" t="n">
-        <v>-58.448523</v>
+        <v>-58.419166</v>
       </c>
       <c r="N396" t="n">
-        <v>-34.62452</v>
+        <v>-34.600265</v>
       </c>
       <c r="O396" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P396" t="inlineStr">
@@ -30029,7 +30029,7 @@
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>-503</t>
+          <t>-504</t>
         </is>
       </c>
       <c r="B397" t="inlineStr">
@@ -30039,17 +30039,17 @@
       </c>
       <c r="C397" t="inlineStr">
         <is>
-          <t>Salguero 842</t>
+          <t>Ohiggins 1611</t>
         </is>
       </c>
       <c r="D397" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E397" t="inlineStr">
         <is>
-          <t>808148673</t>
+          <t>808148679</t>
         </is>
       </c>
       <c r="F397" t="inlineStr">
@@ -30064,7 +30064,7 @@
       </c>
       <c r="H397" t="inlineStr">
         <is>
-          <t>Cambiar columna picada en la base</t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I397" t="n">
@@ -30077,7 +30077,7 @@
       </c>
       <c r="K397" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L397" t="inlineStr">
@@ -30086,51 +30086,51 @@
         </is>
       </c>
       <c r="M397" t="n">
-        <v>-58.419166</v>
+        <v>-58.448993</v>
       </c>
       <c r="N397" t="n">
-        <v>-34.600265</v>
+        <v>-34.564383</v>
       </c>
       <c r="O397" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P397" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>-504</t>
+          <t>-505</t>
         </is>
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C398" t="inlineStr">
         <is>
-          <t>Ohiggins 1611</t>
+          <t>Brasil 3181</t>
         </is>
       </c>
       <c r="D398" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E398" t="inlineStr">
         <is>
-          <t>808148679</t>
+          <t>808150460</t>
         </is>
       </c>
       <c r="F398" t="inlineStr">
         <is>
-          <t>NEW</t>
+          <t>PEBCOM</t>
         </is>
       </c>
       <c r="G398" t="inlineStr">
@@ -30140,7 +30140,7 @@
       </c>
       <c r="H398" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I398" t="n">
@@ -30153,7 +30153,7 @@
       </c>
       <c r="K398" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L398" t="inlineStr">
@@ -30162,26 +30162,26 @@
         </is>
       </c>
       <c r="M398" t="n">
-        <v>-58.448993</v>
+        <v>-58.409002</v>
       </c>
       <c r="N398" t="n">
-        <v>-34.564383</v>
+        <v>-34.634523</v>
       </c>
       <c r="O398" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P398" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t>-505</t>
+          <t>-506</t>
         </is>
       </c>
       <c r="B399" t="inlineStr">
@@ -30191,22 +30191,22 @@
       </c>
       <c r="C399" t="inlineStr">
         <is>
-          <t>Brasil 3181</t>
+          <t>Espinosa 591</t>
         </is>
       </c>
       <c r="D399" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E399" t="inlineStr">
         <is>
-          <t>808150460</t>
+          <t>808150511</t>
         </is>
       </c>
       <c r="F399" t="inlineStr">
         <is>
-          <t>PEBCOM</t>
+          <t>Optical Power</t>
         </is>
       </c>
       <c r="G399" t="inlineStr">
@@ -30229,7 +30229,7 @@
       </c>
       <c r="K399" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L399" t="inlineStr">
@@ -30238,14 +30238,14 @@
         </is>
       </c>
       <c r="M399" t="n">
-        <v>-58.409002</v>
+        <v>-58.449</v>
       </c>
       <c r="N399" t="n">
-        <v>-34.634523</v>
+        <v>-34.616077</v>
       </c>
       <c r="O399" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P399" t="inlineStr">
@@ -30257,32 +30257,32 @@
     <row r="400">
       <c r="A400" t="inlineStr">
         <is>
-          <t>-506</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C400" t="inlineStr">
         <is>
-          <t>Espinosa 591</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D400" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E400" t="inlineStr">
         <is>
-          <t>808150511</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F400" t="inlineStr">
         <is>
-          <t>Optical Power</t>
+          <t>Sin Asignar</t>
         </is>
       </c>
       <c r="G400" t="inlineStr">
@@ -30305,7 +30305,7 @@
       </c>
       <c r="K400" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L400" t="inlineStr">
@@ -30314,26 +30314,26 @@
         </is>
       </c>
       <c r="M400" t="n">
-        <v>-58.449</v>
+        <v>-58.473937</v>
       </c>
       <c r="N400" t="n">
-        <v>-34.616077</v>
+        <v>-34.557355</v>
       </c>
       <c r="O400" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P400" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-508</t>
         </is>
       </c>
       <c r="B401" t="inlineStr">
@@ -30343,7 +30343,7 @@
       </c>
       <c r="C401" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>Moldes 2463</t>
         </is>
       </c>
       <c r="D401" t="inlineStr">
@@ -30353,7 +30353,7 @@
       </c>
       <c r="E401" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>808194234</t>
         </is>
       </c>
       <c r="F401" t="inlineStr">
@@ -30381,7 +30381,7 @@
       </c>
       <c r="K401" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L401" t="inlineStr">
@@ -30390,10 +30390,10 @@
         </is>
       </c>
       <c r="M401" t="n">
-        <v>-58.473937</v>
+        <v>-58.462281</v>
       </c>
       <c r="N401" t="n">
-        <v>-34.557355</v>
+        <v>-34.560321</v>
       </c>
       <c r="O401" t="inlineStr">
         <is>
@@ -30409,7 +30409,7 @@
     <row r="402">
       <c r="A402" t="inlineStr">
         <is>
-          <t>-508</t>
+          <t>-509</t>
         </is>
       </c>
       <c r="B402" t="inlineStr">
@@ -30419,17 +30419,17 @@
       </c>
       <c r="C402" t="inlineStr">
         <is>
-          <t>Moldes 2463</t>
+          <t>Paso 58</t>
         </is>
       </c>
       <c r="D402" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E402" t="inlineStr">
         <is>
-          <t>808194234</t>
+          <t>808194240</t>
         </is>
       </c>
       <c r="F402" t="inlineStr">
@@ -30457,7 +30457,7 @@
       </c>
       <c r="K402" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L402" t="inlineStr">
@@ -30466,26 +30466,26 @@
         </is>
       </c>
       <c r="M402" t="n">
-        <v>-58.462281</v>
+        <v>-58.403422</v>
       </c>
       <c r="N402" t="n">
-        <v>-34.560321</v>
+        <v>-34.609195</v>
       </c>
       <c r="O402" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P402" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>-509</t>
+          <t>-510</t>
         </is>
       </c>
       <c r="B403" t="inlineStr">
@@ -30495,7 +30495,7 @@
       </c>
       <c r="C403" t="inlineStr">
         <is>
-          <t>Paso 58</t>
+          <t>Larrea 590</t>
         </is>
       </c>
       <c r="D403" t="inlineStr">
@@ -30505,7 +30505,7 @@
       </c>
       <c r="E403" t="inlineStr">
         <is>
-          <t>808194240</t>
+          <t>808194254</t>
         </is>
       </c>
       <c r="F403" t="inlineStr">
@@ -30533,7 +30533,7 @@
       </c>
       <c r="K403" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L403" t="inlineStr">
@@ -30542,10 +30542,10 @@
         </is>
       </c>
       <c r="M403" t="n">
-        <v>-58.403422</v>
+        <v>-58.402353</v>
       </c>
       <c r="N403" t="n">
-        <v>-34.609195</v>
+        <v>-34.602205</v>
       </c>
       <c r="O403" t="inlineStr">
         <is>
@@ -30561,7 +30561,7 @@
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>-510</t>
+          <t>6388</t>
         </is>
       </c>
       <c r="B404" t="inlineStr">
@@ -30571,7 +30571,7 @@
       </c>
       <c r="C404" t="inlineStr">
         <is>
-          <t>Larrea 590</t>
+          <t>CASTELLI 304</t>
         </is>
       </c>
       <c r="D404" t="inlineStr">
@@ -30581,12 +30581,12 @@
       </c>
       <c r="E404" t="inlineStr">
         <is>
-          <t>808194254</t>
+          <t>808194260</t>
         </is>
       </c>
       <c r="F404" t="inlineStr">
         <is>
-          <t>Sin Asignar</t>
+          <t>PEBCOM</t>
         </is>
       </c>
       <c r="G404" t="inlineStr">
@@ -30609,7 +30609,7 @@
       </c>
       <c r="K404" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L404" t="inlineStr">
@@ -30618,10 +30618,10 @@
         </is>
       </c>
       <c r="M404" t="n">
-        <v>-58.402353</v>
+        <v>-58.404696</v>
       </c>
       <c r="N404" t="n">
-        <v>-34.602205</v>
+        <v>-34.606337</v>
       </c>
       <c r="O404" t="inlineStr">
         <is>
@@ -30637,7 +30637,7 @@
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>6388</t>
+          <t>6392</t>
         </is>
       </c>
       <c r="B405" t="inlineStr">
@@ -30647,22 +30647,22 @@
       </c>
       <c r="C405" t="inlineStr">
         <is>
-          <t>CASTELLI 304</t>
+          <t>MOLDES 1808</t>
         </is>
       </c>
       <c r="D405" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E405" t="inlineStr">
         <is>
-          <t>808194260</t>
+          <t>808194266</t>
         </is>
       </c>
       <c r="F405" t="inlineStr">
         <is>
-          <t>PEBCOM</t>
+          <t>NEW</t>
         </is>
       </c>
       <c r="G405" t="inlineStr">
@@ -30694,26 +30694,26 @@
         </is>
       </c>
       <c r="M405" t="n">
-        <v>-58.404696</v>
+        <v>-58.45719</v>
       </c>
       <c r="N405" t="n">
-        <v>-34.606337</v>
+        <v>-34.566365</v>
       </c>
       <c r="O405" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P405" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>6392</t>
+          <t>6394</t>
         </is>
       </c>
       <c r="B406" t="inlineStr">
@@ -30723,22 +30723,22 @@
       </c>
       <c r="C406" t="inlineStr">
         <is>
-          <t>MOLDES 1808</t>
+          <t>LAMBARE 1076</t>
         </is>
       </c>
       <c r="D406" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E406" t="inlineStr">
         <is>
-          <t>808194266</t>
+          <t>808194286</t>
         </is>
       </c>
       <c r="F406" t="inlineStr">
         <is>
-          <t>NEW</t>
+          <t>AYKO</t>
         </is>
       </c>
       <c r="G406" t="inlineStr">
@@ -30770,26 +30770,26 @@
         </is>
       </c>
       <c r="M406" t="n">
-        <v>-58.45719</v>
+        <v>-58.43008</v>
       </c>
       <c r="N406" t="n">
-        <v>-34.566365</v>
+        <v>-34.601416</v>
       </c>
       <c r="O406" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P406" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>6394</t>
+          <t>-511</t>
         </is>
       </c>
       <c r="B407" t="inlineStr">
@@ -30799,22 +30799,22 @@
       </c>
       <c r="C407" t="inlineStr">
         <is>
-          <t>LAMBARE 1076</t>
+          <t>Carlos Melo 491</t>
         </is>
       </c>
       <c r="D407" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E407" t="inlineStr">
         <is>
-          <t>808194286</t>
+          <t>808194932</t>
         </is>
       </c>
       <c r="F407" t="inlineStr">
         <is>
-          <t>AYKO</t>
+          <t>Optical Power</t>
         </is>
       </c>
       <c r="G407" t="inlineStr">
@@ -30842,18 +30842,18 @@
       </c>
       <c r="L407" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M407" t="n">
-        <v>-58.43008</v>
+        <v>-58.363292</v>
       </c>
       <c r="N407" t="n">
-        <v>-34.601416</v>
+        <v>-34.642869</v>
       </c>
       <c r="O407" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P407" t="inlineStr">
@@ -30865,32 +30865,32 @@
     <row r="408">
       <c r="A408" t="inlineStr">
         <is>
-          <t>-511</t>
+          <t>-512</t>
         </is>
       </c>
       <c r="B408" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C408" t="inlineStr">
         <is>
-          <t>Carlos Melo 491</t>
+          <t>Ciudad de la Paz 3742</t>
         </is>
       </c>
       <c r="D408" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E408" t="inlineStr">
         <is>
-          <t>808194932</t>
+          <t>808240230</t>
         </is>
       </c>
       <c r="F408" t="inlineStr">
         <is>
-          <t>Optical Power</t>
+          <t>Sin Asignar</t>
         </is>
       </c>
       <c r="G408" t="inlineStr">
@@ -30918,30 +30918,30 @@
       </c>
       <c r="L408" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M408" t="n">
-        <v>-58.363292</v>
+        <v>-58.470347</v>
       </c>
       <c r="N408" t="n">
-        <v>-34.642869</v>
+        <v>-34.547965</v>
       </c>
       <c r="O408" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P408" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t>-512</t>
+          <t>-513</t>
         </is>
       </c>
       <c r="B409" t="inlineStr">
@@ -30951,22 +30951,22 @@
       </c>
       <c r="C409" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 3742</t>
+          <t>Montes de Oca 1809</t>
         </is>
       </c>
       <c r="D409" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E409" t="inlineStr">
         <is>
-          <t>808240230</t>
+          <t>808240768</t>
         </is>
       </c>
       <c r="F409" t="inlineStr">
         <is>
-          <t>Sin Asignar</t>
+          <t>Optical Power</t>
         </is>
       </c>
       <c r="G409" t="inlineStr">
@@ -30976,7 +30976,7 @@
       </c>
       <c r="H409" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna donde esta el monoducto para acceso a edifciio</t>
         </is>
       </c>
       <c r="I409" t="n">
@@ -30998,26 +30998,26 @@
         </is>
       </c>
       <c r="M409" t="n">
-        <v>-58.470347</v>
+        <v>-58.372941</v>
       </c>
       <c r="N409" t="n">
-        <v>-34.547965</v>
+        <v>-34.648341</v>
       </c>
       <c r="O409" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P409" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" t="inlineStr">
         <is>
-          <t>-513</t>
+          <t>-514</t>
         </is>
       </c>
       <c r="B410" t="inlineStr">
@@ -31027,22 +31027,22 @@
       </c>
       <c r="C410" t="inlineStr">
         <is>
-          <t>Montes de Oca 1809</t>
+          <t>Bilbao 2452</t>
         </is>
       </c>
       <c r="D410" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E410" t="inlineStr">
         <is>
-          <t>808240768</t>
+          <t>808243829</t>
         </is>
       </c>
       <c r="F410" t="inlineStr">
         <is>
-          <t>Optical Power</t>
+          <t>Sin Asignar</t>
         </is>
       </c>
       <c r="G410" t="inlineStr">
@@ -31052,7 +31052,7 @@
       </c>
       <c r="H410" t="inlineStr">
         <is>
-          <t>Colocar columna donde esta el monoducto para acceso a edifciio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I410" t="n">
@@ -31074,14 +31074,14 @@
         </is>
       </c>
       <c r="M410" t="n">
-        <v>-58.372941</v>
+        <v>-58.460594</v>
       </c>
       <c r="N410" t="n">
-        <v>-34.648341</v>
+        <v>-34.635581</v>
       </c>
       <c r="O410" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P410" t="inlineStr">
@@ -31093,32 +31093,32 @@
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t>-514</t>
+          <t>6399</t>
         </is>
       </c>
       <c r="B411" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C411" t="inlineStr">
         <is>
-          <t>Bilbao 2452</t>
+          <t>ESCALADA AV. 966</t>
         </is>
       </c>
       <c r="D411" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E411" t="inlineStr">
         <is>
-          <t>808243829</t>
+          <t>808258198</t>
         </is>
       </c>
       <c r="F411" t="inlineStr">
         <is>
-          <t>Sin Asignar</t>
+          <t>AYKO</t>
         </is>
       </c>
       <c r="G411" t="inlineStr">
@@ -31150,46 +31150,46 @@
         </is>
       </c>
       <c r="M411" t="n">
-        <v>-58.460594</v>
+        <v>-58.493069</v>
       </c>
       <c r="N411" t="n">
-        <v>-34.635581</v>
+        <v>-34.646557</v>
       </c>
       <c r="O411" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P411" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>6399</t>
+          <t>-515</t>
         </is>
       </c>
       <c r="B412" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C412" t="inlineStr">
         <is>
-          <t>ESCALADA AV. 966</t>
+          <t>Rivadavia 7470</t>
         </is>
       </c>
       <c r="D412" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E412" t="inlineStr">
         <is>
-          <t>808258198</t>
+          <t>808263485</t>
         </is>
       </c>
       <c r="F412" t="inlineStr">
@@ -31226,93 +31226,17 @@
         </is>
       </c>
       <c r="M412" t="n">
-        <v>-58.493069</v>
+        <v>-58.470715</v>
       </c>
       <c r="N412" t="n">
-        <v>-34.646557</v>
+        <v>-34.631107</v>
       </c>
       <c r="O412" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P412" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="413">
-      <c r="A413" t="inlineStr">
-        <is>
-          <t>-515</t>
-        </is>
-      </c>
-      <c r="B413" t="inlineStr">
-        <is>
-          <t>7/15/2025</t>
-        </is>
-      </c>
-      <c r="C413" t="inlineStr">
-        <is>
-          <t>Rivadavia 7470</t>
-        </is>
-      </c>
-      <c r="D413" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="E413" t="inlineStr">
-        <is>
-          <t>808263485</t>
-        </is>
-      </c>
-      <c r="F413" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G413" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H413" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I413" t="n">
-        <v>1</v>
-      </c>
-      <c r="J413" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K413" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L413" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M413" t="n">
-        <v>-58.470715</v>
-      </c>
-      <c r="N413" t="n">
-        <v>-34.631107</v>
-      </c>
-      <c r="O413" t="inlineStr">
-        <is>
-          <t>Boedo</t>
-        </is>
-      </c>
-      <c r="P413" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>
@@ -53534,7 +53458,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P92"/>
+  <dimension ref="A1:P91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -60211,27 +60135,27 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>-500</t>
+          <t>6394</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Castañares 5656</t>
+          <t>LAMBARE 1076</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>807965768</t>
+          <t>808194286</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -60246,7 +60170,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>Columna chocada con rienda a pique</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I89" t="n">
@@ -60264,18 +60188,18 @@
       </c>
       <c r="L89" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M89" t="n">
-        <v>-58.479921</v>
+        <v>-58.43008</v>
       </c>
       <c r="N89" t="n">
-        <v>-34.673021</v>
+        <v>-34.601416</v>
       </c>
       <c r="O89" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P89" t="inlineStr">
@@ -60287,7 +60211,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>6394</t>
+          <t>6399</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -60297,17 +60221,17 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>LAMBARE 1076</t>
+          <t>ESCALADA AV. 966</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>808194286</t>
+          <t>808258198</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -60344,46 +60268,46 @@
         </is>
       </c>
       <c r="M90" t="n">
-        <v>-58.43008</v>
+        <v>-58.493069</v>
       </c>
       <c r="N90" t="n">
-        <v>-34.601416</v>
+        <v>-34.646557</v>
       </c>
       <c r="O90" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P90" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>6399</t>
+          <t>-515</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>ESCALADA AV. 966</t>
+          <t>Rivadavia 7470</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>808258198</t>
+          <t>808263485</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -60420,93 +60344,17 @@
         </is>
       </c>
       <c r="M91" t="n">
-        <v>-58.493069</v>
+        <v>-58.470715</v>
       </c>
       <c r="N91" t="n">
-        <v>-34.646557</v>
+        <v>-34.631107</v>
       </c>
       <c r="O91" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P91" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>-515</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>7/15/2025</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>Rivadavia 7470</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t>808263485</t>
-        </is>
-      </c>
-      <c r="F92" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H92" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I92" t="n">
-        <v>1</v>
-      </c>
-      <c r="J92" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K92" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L92" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M92" t="n">
-        <v>-58.470715</v>
-      </c>
-      <c r="N92" t="n">
-        <v>-34.631107</v>
-      </c>
-      <c r="O92" t="inlineStr">
-        <is>
-          <t>Boedo</t>
-        </is>
-      </c>
-      <c r="P92" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>